<commit_message>
Cập nhật lần 2
</commit_message>
<xml_diff>
--- a/ProductBacklog_ QL Giao Hàng.xlsx
+++ b/ProductBacklog_ QL Giao Hàng.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tài liệu Word\CNPM NC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7B0787-DED7-4AC1-9F98-A759138D9841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52D4F30-BD8F-48C7-BEAB-5352CBB9BDC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="798" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="798" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Information" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="78">
   <si>
     <t>I. Requirements</t>
   </si>
@@ -202,12 +202,111 @@
 g. cập nhật trạng thái đơn hàng.
 - Trạng thái đơn hàng bao gồm: Chưa nhận, Đã nhận - Chưa giao, Đã nhận – Đang giao và Đã Giao.</t>
   </si>
+  <si>
+    <t>US-01</t>
+  </si>
+  <si>
+    <t>Đăng Nhập</t>
+  </si>
+  <si>
+    <t>Phú</t>
+  </si>
+  <si>
+    <t>23/9/2025</t>
+  </si>
+  <si>
+    <t>30/9/2025</t>
+  </si>
+  <si>
+    <t>Đăng Ký</t>
+  </si>
+  <si>
+    <t>Đăng Xuất</t>
+  </si>
+  <si>
+    <t>Quản lý thông tin</t>
+  </si>
+  <si>
+    <t>Hên</t>
+  </si>
+  <si>
+    <t>Đạt</t>
+  </si>
+  <si>
+    <t>Phát</t>
+  </si>
+  <si>
+    <t>US-02</t>
+  </si>
+  <si>
+    <t>US-03</t>
+  </si>
+  <si>
+    <t>US-04</t>
+  </si>
+  <si>
+    <t>Sprint  2</t>
+  </si>
+  <si>
+    <t>US-05</t>
+  </si>
+  <si>
+    <t>US-06</t>
+  </si>
+  <si>
+    <t>US-07</t>
+  </si>
+  <si>
+    <t>US-08</t>
+  </si>
+  <si>
+    <t>US-09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phát </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Đạt </t>
+  </si>
+  <si>
+    <t>Sprint  3</t>
+  </si>
+  <si>
+    <t>US-10</t>
+  </si>
+  <si>
+    <t>US-11</t>
+  </si>
+  <si>
+    <t>US-12</t>
+  </si>
+  <si>
+    <t>US-13</t>
+  </si>
+  <si>
+    <t>US-14</t>
+  </si>
+  <si>
+    <t>US-15</t>
+  </si>
+  <si>
+    <t>US-16</t>
+  </si>
+  <si>
+    <t>US-17</t>
+  </si>
+  <si>
+    <t>US-18</t>
+  </si>
+  <si>
+    <t>21/10/2025</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -255,8 +354,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -266,12 +370,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="27"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="42"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -294,7 +392,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -434,6 +532,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -442,13 +555,12 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -467,13 +579,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -482,10 +594,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -494,8 +606,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -914,634 +1031,634 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:L46"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A27" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:L46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="31"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="31"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="31"/>
-      <c r="L4" s="31"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="31"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
+      <c r="A5" s="26"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31"/>
+      <c r="A9" s="26"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="31"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="26"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="31"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="31"/>
+      <c r="A12" s="26"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="26"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="31"/>
-      <c r="L13" s="31"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="31"/>
-      <c r="L14" s="31"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
-      <c r="B15" s="31"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="31"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="31"/>
-      <c r="L15" s="31"/>
+      <c r="A15" s="26"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
-      <c r="B16" s="31"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="31"/>
-      <c r="K16" s="31"/>
-      <c r="L16" s="31"/>
+      <c r="A16" s="26"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="31"/>
-      <c r="L17" s="31"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="31"/>
-      <c r="K18" s="31"/>
-      <c r="L18" s="31"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="26"/>
+      <c r="L18" s="26"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="31"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="31"/>
-      <c r="L19" s="31"/>
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="31"/>
-      <c r="B20" s="31"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="31"/>
-      <c r="L20" s="31"/>
+      <c r="A20" s="26"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="26"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="31"/>
-      <c r="B21" s="31"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="31"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="31"/>
-      <c r="L21" s="31"/>
+      <c r="A21" s="26"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="31"/>
-      <c r="B22" s="31"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="31"/>
-      <c r="L22" s="31"/>
+      <c r="A22" s="26"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="26"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="31"/>
-      <c r="B23" s="31"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="31"/>
-      <c r="I23" s="31"/>
-      <c r="J23" s="31"/>
-      <c r="K23" s="31"/>
-      <c r="L23" s="31"/>
+      <c r="A23" s="26"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="26"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="31"/>
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31"/>
-      <c r="J24" s="31"/>
-      <c r="K24" s="31"/>
-      <c r="L24" s="31"/>
+      <c r="A24" s="26"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="26"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="31"/>
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="31"/>
-      <c r="J25" s="31"/>
-      <c r="K25" s="31"/>
-      <c r="L25" s="31"/>
+      <c r="A25" s="26"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="26"/>
+      <c r="L25" s="26"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="31"/>
-      <c r="B26" s="31"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="31"/>
-      <c r="J26" s="31"/>
-      <c r="K26" s="31"/>
-      <c r="L26" s="31"/>
+      <c r="A26" s="26"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="26"/>
+      <c r="K26" s="26"/>
+      <c r="L26" s="26"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="31"/>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
-      <c r="K27" s="31"/>
-      <c r="L27" s="31"/>
+      <c r="A27" s="26"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="26"/>
+      <c r="K27" s="26"/>
+      <c r="L27" s="26"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="31"/>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="31"/>
-      <c r="J28" s="31"/>
-      <c r="K28" s="31"/>
-      <c r="L28" s="31"/>
+      <c r="A28" s="26"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="26"/>
+      <c r="K28" s="26"/>
+      <c r="L28" s="26"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="31"/>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="31"/>
-      <c r="J29" s="31"/>
-      <c r="K29" s="31"/>
-      <c r="L29" s="31"/>
+      <c r="A29" s="26"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
+      <c r="K29" s="26"/>
+      <c r="L29" s="26"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="31"/>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
-      <c r="K30" s="31"/>
-      <c r="L30" s="31"/>
+      <c r="A30" s="26"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
+      <c r="K30" s="26"/>
+      <c r="L30" s="26"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="31"/>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="31"/>
-      <c r="K31" s="31"/>
-      <c r="L31" s="31"/>
+      <c r="A31" s="26"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="26"/>
+      <c r="K31" s="26"/>
+      <c r="L31" s="26"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="31"/>
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="31"/>
-      <c r="J32" s="31"/>
-      <c r="K32" s="31"/>
-      <c r="L32" s="31"/>
+      <c r="A32" s="26"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="26"/>
+      <c r="L32" s="26"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="31"/>
-      <c r="B33" s="31"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="31"/>
-      <c r="H33" s="31"/>
-      <c r="I33" s="31"/>
-      <c r="J33" s="31"/>
-      <c r="K33" s="31"/>
-      <c r="L33" s="31"/>
+      <c r="A33" s="26"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="26"/>
+      <c r="K33" s="26"/>
+      <c r="L33" s="26"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="31"/>
-      <c r="B34" s="31"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="31"/>
-      <c r="I34" s="31"/>
-      <c r="J34" s="31"/>
-      <c r="K34" s="31"/>
-      <c r="L34" s="31"/>
+      <c r="A34" s="26"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="26"/>
+      <c r="J34" s="26"/>
+      <c r="K34" s="26"/>
+      <c r="L34" s="26"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="31"/>
-      <c r="B35" s="31"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="31"/>
-      <c r="G35" s="31"/>
-      <c r="H35" s="31"/>
-      <c r="I35" s="31"/>
-      <c r="J35" s="31"/>
-      <c r="K35" s="31"/>
-      <c r="L35" s="31"/>
+      <c r="A35" s="26"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="26"/>
+      <c r="K35" s="26"/>
+      <c r="L35" s="26"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="31"/>
-      <c r="B36" s="31"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="31"/>
-      <c r="G36" s="31"/>
-      <c r="H36" s="31"/>
-      <c r="I36" s="31"/>
-      <c r="J36" s="31"/>
-      <c r="K36" s="31"/>
-      <c r="L36" s="31"/>
+      <c r="A36" s="26"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="26"/>
+      <c r="K36" s="26"/>
+      <c r="L36" s="26"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="31"/>
-      <c r="B37" s="31"/>
-      <c r="C37" s="31"/>
-      <c r="D37" s="31"/>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
-      <c r="G37" s="31"/>
-      <c r="H37" s="31"/>
-      <c r="I37" s="31"/>
-      <c r="J37" s="31"/>
-      <c r="K37" s="31"/>
-      <c r="L37" s="31"/>
+      <c r="A37" s="26"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="26"/>
+      <c r="G37" s="26"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="26"/>
+      <c r="K37" s="26"/>
+      <c r="L37" s="26"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="31"/>
-      <c r="B38" s="31"/>
-      <c r="C38" s="31"/>
-      <c r="D38" s="31"/>
-      <c r="E38" s="31"/>
-      <c r="F38" s="31"/>
-      <c r="G38" s="31"/>
-      <c r="H38" s="31"/>
-      <c r="I38" s="31"/>
-      <c r="J38" s="31"/>
-      <c r="K38" s="31"/>
-      <c r="L38" s="31"/>
+      <c r="A38" s="26"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="26"/>
+      <c r="J38" s="26"/>
+      <c r="K38" s="26"/>
+      <c r="L38" s="26"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="31"/>
-      <c r="B39" s="31"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="31"/>
-      <c r="H39" s="31"/>
-      <c r="I39" s="31"/>
-      <c r="J39" s="31"/>
-      <c r="K39" s="31"/>
-      <c r="L39" s="31"/>
+      <c r="A39" s="26"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="26"/>
+      <c r="H39" s="26"/>
+      <c r="I39" s="26"/>
+      <c r="J39" s="26"/>
+      <c r="K39" s="26"/>
+      <c r="L39" s="26"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="31"/>
-      <c r="B40" s="31"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="31"/>
-      <c r="H40" s="31"/>
-      <c r="I40" s="31"/>
-      <c r="J40" s="31"/>
-      <c r="K40" s="31"/>
-      <c r="L40" s="31"/>
+      <c r="A40" s="26"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="26"/>
+      <c r="K40" s="26"/>
+      <c r="L40" s="26"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="31"/>
-      <c r="B41" s="31"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="31"/>
-      <c r="H41" s="31"/>
-      <c r="I41" s="31"/>
-      <c r="J41" s="31"/>
-      <c r="K41" s="31"/>
-      <c r="L41" s="31"/>
+      <c r="A41" s="26"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="26"/>
+      <c r="J41" s="26"/>
+      <c r="K41" s="26"/>
+      <c r="L41" s="26"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="31"/>
-      <c r="B42" s="31"/>
-      <c r="C42" s="31"/>
-      <c r="D42" s="31"/>
-      <c r="E42" s="31"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="31"/>
-      <c r="H42" s="31"/>
-      <c r="I42" s="31"/>
-      <c r="J42" s="31"/>
-      <c r="K42" s="31"/>
-      <c r="L42" s="31"/>
+      <c r="A42" s="26"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26"/>
+      <c r="G42" s="26"/>
+      <c r="H42" s="26"/>
+      <c r="I42" s="26"/>
+      <c r="J42" s="26"/>
+      <c r="K42" s="26"/>
+      <c r="L42" s="26"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="31"/>
-      <c r="B43" s="31"/>
-      <c r="C43" s="31"/>
-      <c r="D43" s="31"/>
-      <c r="E43" s="31"/>
-      <c r="F43" s="31"/>
-      <c r="G43" s="31"/>
-      <c r="H43" s="31"/>
-      <c r="I43" s="31"/>
-      <c r="J43" s="31"/>
-      <c r="K43" s="31"/>
-      <c r="L43" s="31"/>
+      <c r="A43" s="26"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="26"/>
+      <c r="G43" s="26"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="26"/>
+      <c r="K43" s="26"/>
+      <c r="L43" s="26"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="31"/>
-      <c r="B44" s="31"/>
-      <c r="C44" s="31"/>
-      <c r="D44" s="31"/>
-      <c r="E44" s="31"/>
-      <c r="F44" s="31"/>
-      <c r="G44" s="31"/>
-      <c r="H44" s="31"/>
-      <c r="I44" s="31"/>
-      <c r="J44" s="31"/>
-      <c r="K44" s="31"/>
-      <c r="L44" s="31"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="26"/>
+      <c r="F44" s="26"/>
+      <c r="G44" s="26"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="26"/>
+      <c r="K44" s="26"/>
+      <c r="L44" s="26"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="31"/>
-      <c r="B45" s="31"/>
-      <c r="C45" s="31"/>
-      <c r="D45" s="31"/>
-      <c r="E45" s="31"/>
-      <c r="F45" s="31"/>
-      <c r="G45" s="31"/>
-      <c r="H45" s="31"/>
-      <c r="I45" s="31"/>
-      <c r="J45" s="31"/>
-      <c r="K45" s="31"/>
-      <c r="L45" s="31"/>
+      <c r="A45" s="26"/>
+      <c r="B45" s="26"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="26"/>
+      <c r="F45" s="26"/>
+      <c r="G45" s="26"/>
+      <c r="H45" s="26"/>
+      <c r="I45" s="26"/>
+      <c r="J45" s="26"/>
+      <c r="K45" s="26"/>
+      <c r="L45" s="26"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="31"/>
-      <c r="B46" s="31"/>
-      <c r="C46" s="31"/>
-      <c r="D46" s="31"/>
-      <c r="E46" s="31"/>
-      <c r="F46" s="31"/>
-      <c r="G46" s="31"/>
-      <c r="H46" s="31"/>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
-      <c r="K46" s="31"/>
-      <c r="L46" s="31"/>
+      <c r="A46" s="26"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="26"/>
+      <c r="F46" s="26"/>
+      <c r="G46" s="26"/>
+      <c r="H46" s="26"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
+      <c r="K46" s="26"/>
+      <c r="L46" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1556,7 +1673,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -1580,106 +1697,106 @@
       <c r="F1" s="27"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="20" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
+      <c r="A4" s="8">
         <v>1</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="20" t="s">
+      <c r="D4" s="8"/>
+      <c r="E4" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="9"/>
+      <c r="F4" s="8"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+      <c r="A5" s="8">
         <v>2</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="20" t="s">
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="9"/>
+      <c r="F5" s="8"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="A6" s="8">
         <v>3</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="20" t="s">
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="9"/>
+      <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
+      <c r="A7" s="8">
         <v>4</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="20" t="s">
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="9"/>
+      <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="9"/>
-    </row>
-    <row r="9" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="22"/>
-    </row>
-    <row r="10" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="22"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="21"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="21"/>
+    </row>
+    <row r="10" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="21"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1696,8 +1813,8 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1708,35 +1825,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="11"/>
+      <c r="B2" s="10"/>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="17" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="12"/>
+      <c r="C4" s="11"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="13"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="12"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -1756,10 +1873,10 @@
       <c r="B7" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="13">
         <v>3</v>
       </c>
-      <c r="G7" s="24"/>
+      <c r="G7" s="23"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -1768,7 +1885,7 @@
       <c r="B8" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="13">
         <v>3</v>
       </c>
     </row>
@@ -1779,7 +1896,7 @@
       <c r="B9" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="13">
         <v>3</v>
       </c>
     </row>
@@ -1790,7 +1907,7 @@
       <c r="B10" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="13">
         <v>5</v>
       </c>
     </row>
@@ -1798,10 +1915,10 @@
       <c r="A11" s="2">
         <v>6</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="13">
         <v>5</v>
       </c>
     </row>
@@ -1812,14 +1929,14 @@
       <c r="B12" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="13">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="13"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="12"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -1828,7 +1945,7 @@
       <c r="B14" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="13">
         <v>8</v>
       </c>
     </row>
@@ -1839,7 +1956,7 @@
       <c r="B15" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C15" s="13">
         <v>8</v>
       </c>
     </row>
@@ -1850,7 +1967,7 @@
       <c r="B16" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="14">
+      <c r="C16" s="13">
         <v>5</v>
       </c>
     </row>
@@ -1861,7 +1978,7 @@
       <c r="B17" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="13">
         <v>5</v>
       </c>
     </row>
@@ -1869,10 +1986,10 @@
       <c r="A18" s="2">
         <v>12</v>
       </c>
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="14">
+      <c r="C18" s="13">
         <v>5</v>
       </c>
     </row>
@@ -1883,14 +2000,14 @@
       <c r="B19" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="14">
+      <c r="C19" s="13">
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="13"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="12"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
@@ -1899,7 +2016,7 @@
       <c r="B21" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="14">
+      <c r="C21" s="13">
         <v>8</v>
       </c>
     </row>
@@ -1910,7 +2027,7 @@
       <c r="B22" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="14">
+      <c r="C22" s="13">
         <v>8</v>
       </c>
     </row>
@@ -1921,7 +2038,7 @@
       <c r="B23" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="14">
+      <c r="C23" s="13">
         <v>5</v>
       </c>
     </row>
@@ -1932,54 +2049,54 @@
       <c r="B24" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="14">
+      <c r="C24" s="13">
         <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="14"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="13"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="13"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="12"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="14"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="13"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="14"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="13"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="14"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="13"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="14"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="13"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="14"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="13"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="13"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="12"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="14"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1991,11 +2108,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6:J6"/>
+      <selection pane="bottomLeft" activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2004,8 +2121,8 @@
     <col min="2" max="2" width="29" customWidth="1"/>
     <col min="3" max="3" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" customWidth="1"/>
     <col min="7" max="7" width="14.44140625" customWidth="1"/>
     <col min="8" max="8" width="13.44140625" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
@@ -2013,204 +2130,581 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="11"/>
+      <c r="B3" s="10"/>
       <c r="E3" s="27"/>
       <c r="F3" s="27"/>
       <c r="G3" s="27"/>
       <c r="H3" s="27"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="19" t="s">
+      <c r="I4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="J4" s="18" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8">
         <f>SUM(C7:C11)</f>
-        <v>0</v>
-      </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
+        <v>12</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
+      <c r="A7" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="8">
+        <v>3</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
+      <c r="A8" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="8">
+        <v>3</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
+      <c r="A9" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="8">
+        <v>3</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
+      <c r="A10" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="8">
+        <v>3</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
+      <c r="A12" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
+      <c r="A13" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="8">
+        <v>5</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="32">
+        <v>45848</v>
+      </c>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
+      <c r="A14" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="8">
+        <v>3</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="32">
+        <v>45848</v>
+      </c>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="8">
+        <v>5</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="32">
+        <v>45848</v>
+      </c>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="8">
+        <v>5</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="32">
+        <v>45848</v>
+      </c>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="8">
+        <v>5</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" s="32">
+        <v>45848</v>
+      </c>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="30"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="8">
+        <v>5</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="32">
+        <v>45848</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="8">
+        <v>3</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="32">
+        <v>45848</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="8">
+        <v>5</v>
+      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="32">
+        <v>45848</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="8">
+        <v>5</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="32">
+        <v>45848</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="8">
+        <v>5</v>
+      </c>
+      <c r="D24" s="8"/>
+      <c r="E24" s="32">
+        <v>45848</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+    </row>
+    <row r="25" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="8">
+        <v>3</v>
+      </c>
+      <c r="D25" s="8"/>
+      <c r="E25" s="32">
+        <v>45848</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+    </row>
+    <row r="26" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="8">
+        <v>3</v>
+      </c>
+      <c r="D26" s="8"/>
+      <c r="E26" s="32">
+        <v>45848</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A14:J14"/>
+  <mergeCells count="6">
+    <mergeCell ref="A19:J19"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="A6:J6"/>
+    <mergeCell ref="A12:J12"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>

<commit_message>
Cập nhật lần 2 (4/11/2025)
</commit_message>
<xml_diff>
--- a/ProductBacklog_ QL Giao Hàng.xlsx
+++ b/ProductBacklog_ QL Giao Hàng.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tài liệu Word\CNPM NC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\GitHub\20_HTQLGH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52D4F30-BD8F-48C7-BEAB-5352CBB9BDC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC65EA2-EC36-47B3-BA95-2CADD7324EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="798" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="798" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Information" sheetId="7" r:id="rId1"/>
@@ -594,18 +594,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -613,6 +601,18 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1043,622 +1043,622 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
+      <c r="A5" s="30"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
+      <c r="A6" s="30"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
+      <c r="A7" s="30"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
+      <c r="A8" s="30"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
+      <c r="A9" s="30"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
+      <c r="A11" s="30"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="26"/>
+      <c r="A13" s="30"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26"/>
+      <c r="A14" s="30"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="26"/>
+      <c r="A15" s="30"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
+      <c r="A16" s="30"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26"/>
+      <c r="A17" s="30"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="26"/>
-      <c r="L18" s="26"/>
+      <c r="A18" s="30"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="26"/>
+      <c r="A19" s="30"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="30"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="26"/>
+      <c r="A20" s="30"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="26"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="26"/>
-      <c r="L21" s="26"/>
+      <c r="A21" s="30"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="26"/>
-      <c r="K22" s="26"/>
-      <c r="L22" s="26"/>
+      <c r="A22" s="30"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="30"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="26"/>
-      <c r="L23" s="26"/>
+      <c r="A23" s="30"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="30"/>
+      <c r="L23" s="30"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="26"/>
+      <c r="A24" s="30"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="30"/>
+      <c r="L24" s="30"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="26"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="26"/>
-      <c r="L25" s="26"/>
+      <c r="A25" s="30"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="30"/>
+      <c r="J25" s="30"/>
+      <c r="K25" s="30"/>
+      <c r="L25" s="30"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="26"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="26"/>
-      <c r="K26" s="26"/>
-      <c r="L26" s="26"/>
+      <c r="A26" s="30"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="30"/>
+      <c r="L26" s="30"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="26"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="26"/>
-      <c r="K27" s="26"/>
-      <c r="L27" s="26"/>
+      <c r="A27" s="30"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="30"/>
+      <c r="L27" s="30"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="26"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="26"/>
-      <c r="J28" s="26"/>
-      <c r="K28" s="26"/>
-      <c r="L28" s="26"/>
+      <c r="A28" s="30"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="30"/>
+      <c r="K28" s="30"/>
+      <c r="L28" s="30"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="26"/>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
-      <c r="K29" s="26"/>
-      <c r="L29" s="26"/>
+      <c r="A29" s="30"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
+      <c r="K29" s="30"/>
+      <c r="L29" s="30"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="26"/>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
-      <c r="K30" s="26"/>
-      <c r="L30" s="26"/>
+      <c r="A30" s="30"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="30"/>
+      <c r="K30" s="30"/>
+      <c r="L30" s="30"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="26"/>
-      <c r="B31" s="26"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="26"/>
-      <c r="K31" s="26"/>
-      <c r="L31" s="26"/>
+      <c r="A31" s="30"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="30"/>
+      <c r="J31" s="30"/>
+      <c r="K31" s="30"/>
+      <c r="L31" s="30"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="26"/>
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="26"/>
-      <c r="H32" s="26"/>
-      <c r="I32" s="26"/>
-      <c r="J32" s="26"/>
-      <c r="K32" s="26"/>
-      <c r="L32" s="26"/>
+      <c r="A32" s="30"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="30"/>
+      <c r="I32" s="30"/>
+      <c r="J32" s="30"/>
+      <c r="K32" s="30"/>
+      <c r="L32" s="30"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="26"/>
-      <c r="B33" s="26"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="26"/>
-      <c r="H33" s="26"/>
-      <c r="I33" s="26"/>
-      <c r="J33" s="26"/>
-      <c r="K33" s="26"/>
-      <c r="L33" s="26"/>
+      <c r="A33" s="30"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="30"/>
+      <c r="J33" s="30"/>
+      <c r="K33" s="30"/>
+      <c r="L33" s="30"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="26"/>
-      <c r="B34" s="26"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="26"/>
-      <c r="J34" s="26"/>
-      <c r="K34" s="26"/>
-      <c r="L34" s="26"/>
+      <c r="A34" s="30"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="30"/>
+      <c r="I34" s="30"/>
+      <c r="J34" s="30"/>
+      <c r="K34" s="30"/>
+      <c r="L34" s="30"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="26"/>
-      <c r="B35" s="26"/>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="26"/>
-      <c r="I35" s="26"/>
-      <c r="J35" s="26"/>
-      <c r="K35" s="26"/>
-      <c r="L35" s="26"/>
+      <c r="A35" s="30"/>
+      <c r="B35" s="30"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="30"/>
+      <c r="I35" s="30"/>
+      <c r="J35" s="30"/>
+      <c r="K35" s="30"/>
+      <c r="L35" s="30"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="26"/>
-      <c r="B36" s="26"/>
-      <c r="C36" s="26"/>
-      <c r="D36" s="26"/>
-      <c r="E36" s="26"/>
-      <c r="F36" s="26"/>
-      <c r="G36" s="26"/>
-      <c r="H36" s="26"/>
-      <c r="I36" s="26"/>
-      <c r="J36" s="26"/>
-      <c r="K36" s="26"/>
-      <c r="L36" s="26"/>
+      <c r="A36" s="30"/>
+      <c r="B36" s="30"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="30"/>
+      <c r="G36" s="30"/>
+      <c r="H36" s="30"/>
+      <c r="I36" s="30"/>
+      <c r="J36" s="30"/>
+      <c r="K36" s="30"/>
+      <c r="L36" s="30"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="26"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="26"/>
-      <c r="F37" s="26"/>
-      <c r="G37" s="26"/>
-      <c r="H37" s="26"/>
-      <c r="I37" s="26"/>
-      <c r="J37" s="26"/>
-      <c r="K37" s="26"/>
-      <c r="L37" s="26"/>
+      <c r="A37" s="30"/>
+      <c r="B37" s="30"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="30"/>
+      <c r="G37" s="30"/>
+      <c r="H37" s="30"/>
+      <c r="I37" s="30"/>
+      <c r="J37" s="30"/>
+      <c r="K37" s="30"/>
+      <c r="L37" s="30"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="26"/>
-      <c r="B38" s="26"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="26"/>
-      <c r="F38" s="26"/>
-      <c r="G38" s="26"/>
-      <c r="H38" s="26"/>
-      <c r="I38" s="26"/>
-      <c r="J38" s="26"/>
-      <c r="K38" s="26"/>
-      <c r="L38" s="26"/>
+      <c r="A38" s="30"/>
+      <c r="B38" s="30"/>
+      <c r="C38" s="30"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="30"/>
+      <c r="G38" s="30"/>
+      <c r="H38" s="30"/>
+      <c r="I38" s="30"/>
+      <c r="J38" s="30"/>
+      <c r="K38" s="30"/>
+      <c r="L38" s="30"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="26"/>
-      <c r="B39" s="26"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="26"/>
-      <c r="H39" s="26"/>
-      <c r="I39" s="26"/>
-      <c r="J39" s="26"/>
-      <c r="K39" s="26"/>
-      <c r="L39" s="26"/>
+      <c r="A39" s="30"/>
+      <c r="B39" s="30"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="30"/>
+      <c r="H39" s="30"/>
+      <c r="I39" s="30"/>
+      <c r="J39" s="30"/>
+      <c r="K39" s="30"/>
+      <c r="L39" s="30"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="26"/>
-      <c r="B40" s="26"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="26"/>
-      <c r="E40" s="26"/>
-      <c r="F40" s="26"/>
-      <c r="G40" s="26"/>
-      <c r="H40" s="26"/>
-      <c r="I40" s="26"/>
-      <c r="J40" s="26"/>
-      <c r="K40" s="26"/>
-      <c r="L40" s="26"/>
+      <c r="A40" s="30"/>
+      <c r="B40" s="30"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="30"/>
+      <c r="G40" s="30"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="30"/>
+      <c r="J40" s="30"/>
+      <c r="K40" s="30"/>
+      <c r="L40" s="30"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="26"/>
-      <c r="B41" s="26"/>
-      <c r="C41" s="26"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="26"/>
-      <c r="G41" s="26"/>
-      <c r="H41" s="26"/>
-      <c r="I41" s="26"/>
-      <c r="J41" s="26"/>
-      <c r="K41" s="26"/>
-      <c r="L41" s="26"/>
+      <c r="A41" s="30"/>
+      <c r="B41" s="30"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="30"/>
+      <c r="E41" s="30"/>
+      <c r="F41" s="30"/>
+      <c r="G41" s="30"/>
+      <c r="H41" s="30"/>
+      <c r="I41" s="30"/>
+      <c r="J41" s="30"/>
+      <c r="K41" s="30"/>
+      <c r="L41" s="30"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="26"/>
-      <c r="B42" s="26"/>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26"/>
-      <c r="G42" s="26"/>
-      <c r="H42" s="26"/>
-      <c r="I42" s="26"/>
-      <c r="J42" s="26"/>
-      <c r="K42" s="26"/>
-      <c r="L42" s="26"/>
+      <c r="A42" s="30"/>
+      <c r="B42" s="30"/>
+      <c r="C42" s="30"/>
+      <c r="D42" s="30"/>
+      <c r="E42" s="30"/>
+      <c r="F42" s="30"/>
+      <c r="G42" s="30"/>
+      <c r="H42" s="30"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
+      <c r="K42" s="30"/>
+      <c r="L42" s="30"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="26"/>
-      <c r="B43" s="26"/>
-      <c r="C43" s="26"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="26"/>
-      <c r="F43" s="26"/>
-      <c r="G43" s="26"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="26"/>
-      <c r="J43" s="26"/>
-      <c r="K43" s="26"/>
-      <c r="L43" s="26"/>
+      <c r="A43" s="30"/>
+      <c r="B43" s="30"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="30"/>
+      <c r="F43" s="30"/>
+      <c r="G43" s="30"/>
+      <c r="H43" s="30"/>
+      <c r="I43" s="30"/>
+      <c r="J43" s="30"/>
+      <c r="K43" s="30"/>
+      <c r="L43" s="30"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="26"/>
-      <c r="F44" s="26"/>
-      <c r="G44" s="26"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="26"/>
-      <c r="K44" s="26"/>
-      <c r="L44" s="26"/>
+      <c r="A44" s="30"/>
+      <c r="B44" s="30"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="30"/>
+      <c r="F44" s="30"/>
+      <c r="G44" s="30"/>
+      <c r="H44" s="30"/>
+      <c r="I44" s="30"/>
+      <c r="J44" s="30"/>
+      <c r="K44" s="30"/>
+      <c r="L44" s="30"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="26"/>
-      <c r="B45" s="26"/>
-      <c r="C45" s="26"/>
-      <c r="D45" s="26"/>
-      <c r="E45" s="26"/>
-      <c r="F45" s="26"/>
-      <c r="G45" s="26"/>
-      <c r="H45" s="26"/>
-      <c r="I45" s="26"/>
-      <c r="J45" s="26"/>
-      <c r="K45" s="26"/>
-      <c r="L45" s="26"/>
+      <c r="A45" s="30"/>
+      <c r="B45" s="30"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="30"/>
+      <c r="F45" s="30"/>
+      <c r="G45" s="30"/>
+      <c r="H45" s="30"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
+      <c r="K45" s="30"/>
+      <c r="L45" s="30"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="26"/>
-      <c r="B46" s="26"/>
-      <c r="C46" s="26"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="26"/>
-      <c r="F46" s="26"/>
-      <c r="G46" s="26"/>
-      <c r="H46" s="26"/>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
-      <c r="K46" s="26"/>
-      <c r="L46" s="26"/>
+      <c r="A46" s="30"/>
+      <c r="B46" s="30"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="30"/>
+      <c r="G46" s="30"/>
+      <c r="H46" s="30"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
+      <c r="K46" s="30"/>
+      <c r="L46" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1687,14 +1687,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
@@ -1812,8 +1812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -2110,7 +2110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="N8" sqref="N8"/>
     </sheetView>
@@ -2130,18 +2130,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
     </row>
     <row r="2" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
@@ -2155,10 +2155,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="10"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
@@ -2208,18 +2208,18 @@
       <c r="J5" s="8"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
@@ -2330,24 +2330,24 @@
       <c r="J11" s="8"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="27" t="s">
         <v>21</v>
       </c>
       <c r="C13" s="8">
@@ -2359,7 +2359,7 @@
       <c r="E13" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="32">
+      <c r="F13" s="28">
         <v>45848</v>
       </c>
       <c r="G13" s="8"/>
@@ -2371,7 +2371,7 @@
       <c r="A14" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="27" t="s">
         <v>26</v>
       </c>
       <c r="C14" s="8">
@@ -2383,7 +2383,7 @@
       <c r="E14" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="F14" s="32">
+      <c r="F14" s="28">
         <v>45848</v>
       </c>
       <c r="G14" s="19"/>
@@ -2395,7 +2395,7 @@
       <c r="A15" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="27" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="8">
@@ -2407,7 +2407,7 @@
       <c r="E15" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="32">
+      <c r="F15" s="28">
         <v>45848</v>
       </c>
       <c r="G15" s="8"/>
@@ -2431,7 +2431,7 @@
       <c r="E16" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="F16" s="32">
+      <c r="F16" s="28">
         <v>45848</v>
       </c>
       <c r="G16" s="8"/>
@@ -2455,7 +2455,7 @@
       <c r="E17" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="F17" s="32">
+      <c r="F17" s="28">
         <v>45848</v>
       </c>
       <c r="G17" s="8"/>
@@ -2464,7 +2464,7 @@
       <c r="J17" s="8"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
+      <c r="A18" s="26"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
@@ -2476,18 +2476,18 @@
       <c r="J18" s="8"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="29"/>
-      <c r="J19" s="29"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="32"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
@@ -2500,7 +2500,7 @@
         <v>5</v>
       </c>
       <c r="D20" s="8"/>
-      <c r="E20" s="32">
+      <c r="E20" s="28">
         <v>45848</v>
       </c>
       <c r="F20" s="8" t="s">
@@ -2522,7 +2522,7 @@
         <v>3</v>
       </c>
       <c r="D21" s="8"/>
-      <c r="E21" s="32">
+      <c r="E21" s="28">
         <v>45848</v>
       </c>
       <c r="F21" s="8" t="s">
@@ -2544,7 +2544,7 @@
         <v>5</v>
       </c>
       <c r="D22" s="8"/>
-      <c r="E22" s="32">
+      <c r="E22" s="28">
         <v>45848</v>
       </c>
       <c r="F22" s="8" t="s">
@@ -2566,7 +2566,7 @@
         <v>5</v>
       </c>
       <c r="D23" s="8"/>
-      <c r="E23" s="32">
+      <c r="E23" s="28">
         <v>45848</v>
       </c>
       <c r="F23" s="8" t="s">
@@ -2588,7 +2588,7 @@
         <v>5</v>
       </c>
       <c r="D24" s="8"/>
-      <c r="E24" s="32">
+      <c r="E24" s="28">
         <v>45848</v>
       </c>
       <c r="F24" s="8" t="s">
@@ -2610,7 +2610,7 @@
         <v>3</v>
       </c>
       <c r="D25" s="8"/>
-      <c r="E25" s="32">
+      <c r="E25" s="28">
         <v>45848</v>
       </c>
       <c r="F25" s="8" t="s">
@@ -2625,14 +2625,14 @@
       <c r="A26" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B26" s="33" t="s">
+      <c r="B26" s="29" t="s">
         <v>37</v>
       </c>
       <c r="C26" s="8">
         <v>3</v>
       </c>
       <c r="D26" s="8"/>
-      <c r="E26" s="32">
+      <c r="E26" s="28">
         <v>45848</v>
       </c>
       <c r="F26" s="8" t="s">

</xml_diff>